<commit_message>
Rollenbeheer verbouwd naar structuur met ISA. Dat werkt echter niet. Zie issue 237
</commit_message>
<xml_diff>
--- a/MDT/Autorisaties.xlsx
+++ b/MDT/Autorisaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="636" yWindow="660" windowWidth="23256" windowHeight="11892" activeTab="6"/>
+    <workbookView xWindow="636" yWindow="660" windowWidth="23256" windowHeight="11892" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bevoegdheid" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
   <si>
     <t>Bevoegdheid</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Beheren rollenpassen</t>
   </si>
   <si>
-    <t>beheerderVan</t>
-  </si>
-  <si>
     <t>[Dienst]</t>
   </si>
   <si>
@@ -371,6 +368,15 @@
   </si>
   <si>
     <t>121;122;123;124;125</t>
+  </si>
+  <si>
+    <t>beheerderVan~</t>
+  </si>
+  <si>
+    <t>Beheerder</t>
+  </si>
+  <si>
+    <t>Rol</t>
   </si>
 </sst>
 </file>
@@ -9778,8 +9784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9799,7 +9805,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
@@ -9816,7 +9822,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -10184,10 +10190,10 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -12011,7 +12017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -12022,79 +12028,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
         <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
         <v>114</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Rollenbeheer verbouwd naar structuur met ISA. Dat werkt echter niet. Zie issue 237"
This reverts commit d18253e2f09e42758df53373552d5496fe510c89.
</commit_message>
<xml_diff>
--- a/MDT/Autorisaties.xlsx
+++ b/MDT/Autorisaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="636" yWindow="660" windowWidth="23256" windowHeight="11892" activeTab="1"/>
+    <workbookView xWindow="636" yWindow="660" windowWidth="23256" windowHeight="11892" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Bevoegdheid" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
   <si>
     <t>Bevoegdheid</t>
   </si>
@@ -310,6 +310,9 @@
     <t>Beheren rollenpassen</t>
   </si>
   <si>
+    <t>beheerderVan</t>
+  </si>
+  <si>
     <t>[Dienst]</t>
   </si>
   <si>
@@ -368,15 +371,6 @@
   </si>
   <si>
     <t>121;122;123;124;125</t>
-  </si>
-  <si>
-    <t>beheerderVan~</t>
-  </si>
-  <si>
-    <t>Beheerder</t>
-  </si>
-  <si>
-    <t>Rol</t>
   </si>
 </sst>
 </file>
@@ -9784,8 +9778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9805,7 +9799,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
@@ -9822,7 +9816,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -10190,10 +10184,10 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -12017,7 +12011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -12028,79 +12022,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>